<commit_message>
Implemented and tested ability to set relations that already exist in DAVIE to inactive instead of deleting them.
Also keeps all inactive relations that were manually added to the validated documents by the user
</commit_message>
<xml_diff>
--- a/UnitTests/project_files_test/OTLWizardProjects/reference_files/ref_add_remove_test.xlsx
+++ b/UnitTests/project_files_test/OTLWizardProjects/reference_files/ref_add_remove_test.xlsx
@@ -1647,45 +1647,97 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>dummy_bevestiging_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>dummy_zQp</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Pictogram</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>dummy_a</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>dummy_okopD</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Funderingsmassief</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>dummy_TyBGmXfXC</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>dummy_dY</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Bevestiging</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>dummy_bevestiging_2</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>dummy_zQp</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>dummy_Ej</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>dummy_Q</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>dummy_okopD</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>dummy_tCIvXsNGzb</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>dummy_bcjseEAj</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>dummy_dY</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>False</t>
         </is>
@@ -1769,27 +1821,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dummy_hoort_bij</t>
+          <t>dummy_C_-_dummy_hxOTHWe_-_HoortBij</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dummy_LxexRM</t>
+          <t>OTLMOW</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Verkeersbordsteun</t>
+          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Pictogram</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>dummy_vbeo</t>
+          <t>dummy_C</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>dummy_Ouee</t>
+          <t>dummy_Ek</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1799,12 +1851,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>dummy_LGG</t>
+          <t>dummy_hxOTHWe</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>dummy_ZT</t>
+          <t>dummy_GfaE</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1812,54 +1864,6 @@
           <t>True</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#HoortBij</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>dummy_C_-_dummy_hxOTHWe_-_HoortBij</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>OTLMOW</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/onderdeel#Pictogram</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>dummy_C</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>dummy_Ek</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://wegenenverkeer.data.vlaanderen.be/ns/installatie#Verkeersbordopstelling</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>dummy_hxOTHWe</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>dummy_GfaE</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>